<commit_message>
partial progress on #56 NOT TESTED
</commit_message>
<xml_diff>
--- a/src/technology/widget56/widget56.xlsx
+++ b/src/technology/widget56/widget56.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rhanes\GitHub\tyche\src\technology\widget63\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rhanes\GitHub\tyche\src\technology\widget56\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1370A473-0D66-41A5-887D-B336C43CF461}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27C1939C-DEFB-4B54-B2D0-A7A10E88B7AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7185" yWindow="2190" windowWidth="16020" windowHeight="13155" xr2:uid="{A613468B-4246-47D0-8059-797BD75C3238}"/>
+    <workbookView xWindow="28680" yWindow="-7380" windowWidth="16440" windowHeight="29040" xr2:uid="{A613468B-4246-47D0-8059-797BD75C3238}"/>
   </bookViews>
   <sheets>
     <sheet name="designs" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2078" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2073" uniqueCount="124">
   <si>
     <t>Technology</t>
   </si>
@@ -765,10 +765,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{404BF247-5429-4E4B-9678-6277797CABB5}">
-  <dimension ref="A1:G183"/>
+  <dimension ref="A1:G182"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A66" sqref="A66:XFD66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2186,7 +2186,7 @@
         <v>10</v>
       </c>
       <c r="D66" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E66">
         <v>30</v>
@@ -2206,7 +2206,7 @@
         <v>10</v>
       </c>
       <c r="D67" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E67">
         <v>30</v>
@@ -2223,16 +2223,19 @@
         <v>43</v>
       </c>
       <c r="C68" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D68" t="s">
-        <v>32</v>
-      </c>
-      <c r="E68">
-        <v>30</v>
-      </c>
-      <c r="F68" t="s">
-        <v>28</v>
+        <v>33</v>
+      </c>
+      <c r="E68" t="s">
+        <v>44</v>
+      </c>
+      <c r="F68">
+        <v>1</v>
+      </c>
+      <c r="G68" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -2243,19 +2246,19 @@
         <v>43</v>
       </c>
       <c r="C69" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D69" t="s">
         <v>33</v>
       </c>
-      <c r="E69" t="s">
-        <v>44</v>
-      </c>
-      <c r="F69">
-        <v>1</v>
+      <c r="E69">
+        <v>2.15</v>
+      </c>
+      <c r="F69" t="s">
+        <v>34</v>
       </c>
       <c r="G69" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
@@ -2266,19 +2269,16 @@
         <v>43</v>
       </c>
       <c r="C70" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D70" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E70">
-        <v>2.15</v>
+        <v>1</v>
       </c>
       <c r="F70" t="s">
-        <v>34</v>
-      </c>
-      <c r="G70" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
@@ -2286,19 +2286,22 @@
         <v>14</v>
       </c>
       <c r="B71" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C71" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D71" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="E71">
-        <v>1</v>
+        <v>771750</v>
       </c>
       <c r="F71" t="s">
-        <v>36</v>
+        <v>17</v>
+      </c>
+      <c r="G71" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -2312,16 +2315,16 @@
         <v>7</v>
       </c>
       <c r="D72" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E72">
-        <v>771750</v>
+        <v>10352316240</v>
       </c>
       <c r="F72" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G72" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -2332,19 +2335,19 @@
         <v>45</v>
       </c>
       <c r="C73" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D73" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E73">
-        <v>10352316240</v>
-      </c>
-      <c r="F73" t="s">
-        <v>20</v>
+        <v>0.8</v>
+      </c>
+      <c r="F73">
+        <v>1</v>
       </c>
       <c r="G73" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -2358,16 +2361,16 @@
         <v>8</v>
       </c>
       <c r="D74" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E74">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="F74">
         <v>1</v>
       </c>
       <c r="G74" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -2378,19 +2381,19 @@
         <v>45</v>
       </c>
       <c r="C75" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D75" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E75">
-        <v>1</v>
-      </c>
-      <c r="F75">
-        <v>1</v>
+        <v>58</v>
+      </c>
+      <c r="F75" t="s">
+        <v>24</v>
       </c>
       <c r="G75" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
@@ -2404,16 +2407,13 @@
         <v>9</v>
       </c>
       <c r="D76" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E76">
-        <v>58</v>
+        <v>5.2100000000000002E-3</v>
       </c>
       <c r="F76" t="s">
-        <v>24</v>
-      </c>
-      <c r="G76" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -2424,16 +2424,16 @@
         <v>45</v>
       </c>
       <c r="C77" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D77" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="E77">
-        <v>5.2100000000000002E-3</v>
+        <v>30</v>
       </c>
       <c r="F77" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
@@ -2447,7 +2447,7 @@
         <v>10</v>
       </c>
       <c r="D78" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E78">
         <v>30</v>
@@ -2467,7 +2467,7 @@
         <v>10</v>
       </c>
       <c r="D79" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E79">
         <v>30</v>
@@ -2487,7 +2487,7 @@
         <v>10</v>
       </c>
       <c r="D80" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E80">
         <v>30</v>
@@ -2507,7 +2507,7 @@
         <v>10</v>
       </c>
       <c r="D81" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E81">
         <v>30</v>
@@ -2524,16 +2524,19 @@
         <v>45</v>
       </c>
       <c r="C82" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D82" t="s">
-        <v>32</v>
-      </c>
-      <c r="E82">
-        <v>30</v>
-      </c>
-      <c r="F82" t="s">
-        <v>28</v>
+        <v>33</v>
+      </c>
+      <c r="E82" t="s">
+        <v>46</v>
+      </c>
+      <c r="F82">
+        <v>1</v>
+      </c>
+      <c r="G82" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -2544,19 +2547,19 @@
         <v>45</v>
       </c>
       <c r="C83" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D83" t="s">
         <v>33</v>
       </c>
-      <c r="E83" t="s">
-        <v>46</v>
-      </c>
-      <c r="F83">
-        <v>1</v>
+      <c r="E83">
+        <v>2.15</v>
+      </c>
+      <c r="F83" t="s">
+        <v>34</v>
       </c>
       <c r="G83" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
@@ -2567,19 +2570,16 @@
         <v>45</v>
       </c>
       <c r="C84" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D84" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E84">
-        <v>2.15</v>
+        <v>1</v>
       </c>
       <c r="F84" t="s">
-        <v>34</v>
-      </c>
-      <c r="G84" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
@@ -2587,19 +2587,22 @@
         <v>14</v>
       </c>
       <c r="B85" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C85" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D85" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="E85">
-        <v>1</v>
+        <v>771750</v>
       </c>
       <c r="F85" t="s">
-        <v>36</v>
+        <v>17</v>
+      </c>
+      <c r="G85" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -2613,16 +2616,16 @@
         <v>7</v>
       </c>
       <c r="D86" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E86">
-        <v>771750</v>
+        <v>9718500960</v>
       </c>
       <c r="F86" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G86" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
@@ -2633,19 +2636,19 @@
         <v>47</v>
       </c>
       <c r="C87" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D87" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E87">
-        <v>9718500960</v>
-      </c>
-      <c r="F87" t="s">
-        <v>20</v>
+        <v>0.8</v>
+      </c>
+      <c r="F87">
+        <v>1</v>
       </c>
       <c r="G87" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -2659,16 +2662,16 @@
         <v>8</v>
       </c>
       <c r="D88" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E88">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="F88">
         <v>1</v>
       </c>
       <c r="G88" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
@@ -2679,19 +2682,19 @@
         <v>47</v>
       </c>
       <c r="C89" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D89" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E89">
-        <v>1</v>
-      </c>
-      <c r="F89">
-        <v>1</v>
+        <v>58</v>
+      </c>
+      <c r="F89" t="s">
+        <v>24</v>
       </c>
       <c r="G89" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
@@ -2705,16 +2708,13 @@
         <v>9</v>
       </c>
       <c r="D90" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E90">
-        <v>58</v>
+        <v>5.2100000000000002E-3</v>
       </c>
       <c r="F90" t="s">
-        <v>24</v>
-      </c>
-      <c r="G90" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
@@ -2725,16 +2725,16 @@
         <v>47</v>
       </c>
       <c r="C91" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D91" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="E91">
-        <v>5.2100000000000002E-3</v>
+        <v>30</v>
       </c>
       <c r="F91" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
@@ -2748,7 +2748,7 @@
         <v>10</v>
       </c>
       <c r="D92" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E92">
         <v>30</v>
@@ -2768,7 +2768,7 @@
         <v>10</v>
       </c>
       <c r="D93" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E93">
         <v>30</v>
@@ -2788,7 +2788,7 @@
         <v>10</v>
       </c>
       <c r="D94" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E94">
         <v>30</v>
@@ -2808,7 +2808,7 @@
         <v>10</v>
       </c>
       <c r="D95" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E95">
         <v>30</v>
@@ -2825,16 +2825,19 @@
         <v>47</v>
       </c>
       <c r="C96" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D96" t="s">
-        <v>32</v>
-      </c>
-      <c r="E96">
-        <v>30</v>
-      </c>
-      <c r="F96" t="s">
-        <v>28</v>
+        <v>33</v>
+      </c>
+      <c r="E96" t="s">
+        <v>48</v>
+      </c>
+      <c r="F96">
+        <v>1</v>
+      </c>
+      <c r="G96" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
@@ -2845,19 +2848,19 @@
         <v>47</v>
       </c>
       <c r="C97" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D97" t="s">
         <v>33</v>
       </c>
-      <c r="E97" t="s">
-        <v>48</v>
-      </c>
-      <c r="F97">
-        <v>1</v>
+      <c r="E97">
+        <v>2.15</v>
+      </c>
+      <c r="F97" t="s">
+        <v>34</v>
       </c>
       <c r="G97" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
@@ -2868,19 +2871,16 @@
         <v>47</v>
       </c>
       <c r="C98" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D98" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E98">
-        <v>2.15</v>
+        <v>1</v>
       </c>
       <c r="F98" t="s">
-        <v>34</v>
-      </c>
-      <c r="G98" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
@@ -2888,19 +2888,22 @@
         <v>14</v>
       </c>
       <c r="B99" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C99" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D99" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="E99">
-        <v>1</v>
+        <v>771750</v>
       </c>
       <c r="F99" t="s">
-        <v>36</v>
+        <v>17</v>
+      </c>
+      <c r="G99" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
@@ -2914,16 +2917,16 @@
         <v>7</v>
       </c>
       <c r="D100" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E100">
-        <v>771750</v>
+        <v>10563588000</v>
       </c>
       <c r="F100" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G100" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
@@ -2934,19 +2937,19 @@
         <v>49</v>
       </c>
       <c r="C101" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D101" t="s">
-        <v>19</v>
-      </c>
-      <c r="E101">
-        <v>10563588000</v>
-      </c>
-      <c r="F101" t="s">
-        <v>20</v>
+        <v>16</v>
+      </c>
+      <c r="E101" t="s">
+        <v>50</v>
+      </c>
+      <c r="F101">
+        <v>1</v>
       </c>
       <c r="G101" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
@@ -2960,16 +2963,16 @@
         <v>8</v>
       </c>
       <c r="D102" t="s">
-        <v>16</v>
-      </c>
-      <c r="E102" t="s">
-        <v>50</v>
+        <v>19</v>
+      </c>
+      <c r="E102">
+        <v>1</v>
       </c>
       <c r="F102">
         <v>1</v>
       </c>
       <c r="G102" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
@@ -2980,19 +2983,19 @@
         <v>49</v>
       </c>
       <c r="C103" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D103" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E103">
-        <v>1</v>
-      </c>
-      <c r="F103">
-        <v>1</v>
+        <v>58</v>
+      </c>
+      <c r="F103" t="s">
+        <v>24</v>
       </c>
       <c r="G103" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
@@ -3006,16 +3009,13 @@
         <v>9</v>
       </c>
       <c r="D104" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E104">
-        <v>58</v>
+        <v>5.2100000000000002E-3</v>
       </c>
       <c r="F104" t="s">
-        <v>24</v>
-      </c>
-      <c r="G104" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
@@ -3026,16 +3026,16 @@
         <v>49</v>
       </c>
       <c r="C105" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D105" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="E105">
-        <v>5.2100000000000002E-3</v>
+        <v>30</v>
       </c>
       <c r="F105" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
@@ -3049,7 +3049,7 @@
         <v>10</v>
       </c>
       <c r="D106" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E106">
         <v>30</v>
@@ -3069,7 +3069,7 @@
         <v>10</v>
       </c>
       <c r="D107" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E107">
         <v>30</v>
@@ -3089,7 +3089,7 @@
         <v>10</v>
       </c>
       <c r="D108" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E108">
         <v>30</v>
@@ -3109,7 +3109,7 @@
         <v>10</v>
       </c>
       <c r="D109" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E109">
         <v>30</v>
@@ -3126,16 +3126,19 @@
         <v>49</v>
       </c>
       <c r="C110" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D110" t="s">
-        <v>32</v>
-      </c>
-      <c r="E110">
-        <v>30</v>
-      </c>
-      <c r="F110" t="s">
-        <v>28</v>
+        <v>33</v>
+      </c>
+      <c r="E110" t="s">
+        <v>51</v>
+      </c>
+      <c r="F110">
+        <v>1</v>
+      </c>
+      <c r="G110" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
@@ -3146,19 +3149,19 @@
         <v>49</v>
       </c>
       <c r="C111" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D111" t="s">
         <v>33</v>
       </c>
-      <c r="E111" t="s">
-        <v>51</v>
-      </c>
-      <c r="F111">
-        <v>1</v>
+      <c r="E111">
+        <v>2.15</v>
+      </c>
+      <c r="F111" t="s">
+        <v>34</v>
       </c>
       <c r="G111" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
@@ -3169,19 +3172,16 @@
         <v>49</v>
       </c>
       <c r="C112" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D112" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E112">
-        <v>2.15</v>
+        <v>1</v>
       </c>
       <c r="F112" t="s">
-        <v>34</v>
-      </c>
-      <c r="G112" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
@@ -3189,19 +3189,22 @@
         <v>14</v>
       </c>
       <c r="B113" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C113" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D113" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="E113">
-        <v>1</v>
+        <v>771750</v>
       </c>
       <c r="F113" t="s">
-        <v>36</v>
+        <v>17</v>
+      </c>
+      <c r="G113" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
@@ -3215,16 +3218,16 @@
         <v>7</v>
       </c>
       <c r="D114" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E114">
-        <v>771750</v>
+        <v>10563588000</v>
       </c>
       <c r="F114" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G114" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
@@ -3235,19 +3238,19 @@
         <v>52</v>
       </c>
       <c r="C115" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D115" t="s">
-        <v>19</v>
-      </c>
-      <c r="E115">
-        <v>10563588000</v>
-      </c>
-      <c r="F115" t="s">
-        <v>20</v>
+        <v>16</v>
+      </c>
+      <c r="E115" t="s">
+        <v>53</v>
+      </c>
+      <c r="F115">
+        <v>1</v>
       </c>
       <c r="G115" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
@@ -3261,16 +3264,16 @@
         <v>8</v>
       </c>
       <c r="D116" t="s">
-        <v>16</v>
-      </c>
-      <c r="E116" t="s">
-        <v>53</v>
+        <v>19</v>
+      </c>
+      <c r="E116">
+        <v>1</v>
       </c>
       <c r="F116">
         <v>1</v>
       </c>
       <c r="G116" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
@@ -3281,19 +3284,19 @@
         <v>52</v>
       </c>
       <c r="C117" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D117" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E117">
-        <v>1</v>
-      </c>
-      <c r="F117">
-        <v>1</v>
+        <v>58</v>
+      </c>
+      <c r="F117" t="s">
+        <v>24</v>
       </c>
       <c r="G117" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
@@ -3307,16 +3310,13 @@
         <v>9</v>
       </c>
       <c r="D118" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E118">
-        <v>58</v>
+        <v>5.2100000000000002E-3</v>
       </c>
       <c r="F118" t="s">
-        <v>24</v>
-      </c>
-      <c r="G118" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
@@ -3327,16 +3327,16 @@
         <v>52</v>
       </c>
       <c r="C119" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D119" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="E119">
-        <v>5.2100000000000002E-3</v>
+        <v>30</v>
       </c>
       <c r="F119" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
@@ -3350,7 +3350,7 @@
         <v>10</v>
       </c>
       <c r="D120" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E120">
         <v>30</v>
@@ -3370,7 +3370,7 @@
         <v>10</v>
       </c>
       <c r="D121" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E121">
         <v>30</v>
@@ -3390,7 +3390,7 @@
         <v>10</v>
       </c>
       <c r="D122" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E122">
         <v>30</v>
@@ -3410,7 +3410,7 @@
         <v>10</v>
       </c>
       <c r="D123" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E123">
         <v>30</v>
@@ -3427,16 +3427,19 @@
         <v>52</v>
       </c>
       <c r="C124" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D124" t="s">
-        <v>32</v>
-      </c>
-      <c r="E124">
-        <v>30</v>
-      </c>
-      <c r="F124" t="s">
-        <v>28</v>
+        <v>33</v>
+      </c>
+      <c r="E124" t="s">
+        <v>54</v>
+      </c>
+      <c r="F124">
+        <v>1</v>
+      </c>
+      <c r="G124" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
@@ -3447,19 +3450,19 @@
         <v>52</v>
       </c>
       <c r="C125" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D125" t="s">
         <v>33</v>
       </c>
-      <c r="E125" t="s">
-        <v>54</v>
-      </c>
-      <c r="F125">
-        <v>1</v>
+      <c r="E125">
+        <v>2.15</v>
+      </c>
+      <c r="F125" t="s">
+        <v>34</v>
       </c>
       <c r="G125" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
@@ -3470,19 +3473,16 @@
         <v>52</v>
       </c>
       <c r="C126" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D126" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E126">
-        <v>2.15</v>
+        <v>1</v>
       </c>
       <c r="F126" t="s">
-        <v>34</v>
-      </c>
-      <c r="G126" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
@@ -3490,19 +3490,22 @@
         <v>14</v>
       </c>
       <c r="B127" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C127" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D127" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="E127">
-        <v>1</v>
+        <v>771750</v>
       </c>
       <c r="F127" t="s">
-        <v>36</v>
+        <v>17</v>
+      </c>
+      <c r="G127" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
@@ -3516,16 +3519,16 @@
         <v>7</v>
       </c>
       <c r="D128" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E128">
-        <v>771750</v>
+        <v>10563588000</v>
       </c>
       <c r="F128" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G128" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
@@ -3536,19 +3539,19 @@
         <v>55</v>
       </c>
       <c r="C129" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D129" t="s">
-        <v>19</v>
-      </c>
-      <c r="E129">
-        <v>10563588000</v>
-      </c>
-      <c r="F129" t="s">
-        <v>20</v>
+        <v>16</v>
+      </c>
+      <c r="E129" t="s">
+        <v>56</v>
+      </c>
+      <c r="F129">
+        <v>1</v>
       </c>
       <c r="G129" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
@@ -3562,16 +3565,16 @@
         <v>8</v>
       </c>
       <c r="D130" t="s">
-        <v>16</v>
-      </c>
-      <c r="E130" t="s">
-        <v>56</v>
+        <v>19</v>
+      </c>
+      <c r="E130">
+        <v>1</v>
       </c>
       <c r="F130">
         <v>1</v>
       </c>
       <c r="G130" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
@@ -3582,19 +3585,19 @@
         <v>55</v>
       </c>
       <c r="C131" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D131" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E131">
-        <v>1</v>
-      </c>
-      <c r="F131">
-        <v>1</v>
+        <v>58</v>
+      </c>
+      <c r="F131" t="s">
+        <v>24</v>
       </c>
       <c r="G131" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
@@ -3608,16 +3611,13 @@
         <v>9</v>
       </c>
       <c r="D132" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E132">
-        <v>58</v>
+        <v>5.2100000000000002E-3</v>
       </c>
       <c r="F132" t="s">
-        <v>24</v>
-      </c>
-      <c r="G132" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
@@ -3628,16 +3628,16 @@
         <v>55</v>
       </c>
       <c r="C133" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D133" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="E133">
-        <v>5.2100000000000002E-3</v>
+        <v>30</v>
       </c>
       <c r="F133" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
@@ -3651,7 +3651,7 @@
         <v>10</v>
       </c>
       <c r="D134" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E134">
         <v>30</v>
@@ -3671,7 +3671,7 @@
         <v>10</v>
       </c>
       <c r="D135" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E135">
         <v>30</v>
@@ -3691,7 +3691,7 @@
         <v>10</v>
       </c>
       <c r="D136" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E136">
         <v>30</v>
@@ -3711,7 +3711,7 @@
         <v>10</v>
       </c>
       <c r="D137" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E137">
         <v>30</v>
@@ -3728,16 +3728,19 @@
         <v>55</v>
       </c>
       <c r="C138" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D138" t="s">
-        <v>32</v>
-      </c>
-      <c r="E138">
-        <v>30</v>
-      </c>
-      <c r="F138" t="s">
-        <v>28</v>
+        <v>33</v>
+      </c>
+      <c r="E138" t="s">
+        <v>46</v>
+      </c>
+      <c r="F138">
+        <v>1</v>
+      </c>
+      <c r="G138" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
@@ -3748,19 +3751,19 @@
         <v>55</v>
       </c>
       <c r="C139" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D139" t="s">
         <v>33</v>
       </c>
-      <c r="E139" t="s">
-        <v>46</v>
-      </c>
-      <c r="F139">
-        <v>1</v>
+      <c r="E139">
+        <v>2.15</v>
+      </c>
+      <c r="F139" t="s">
+        <v>34</v>
       </c>
       <c r="G139" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
@@ -3771,19 +3774,16 @@
         <v>55</v>
       </c>
       <c r="C140" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D140" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E140">
-        <v>2.15</v>
+        <v>1</v>
       </c>
       <c r="F140" t="s">
-        <v>34</v>
-      </c>
-      <c r="G140" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
@@ -3791,19 +3791,22 @@
         <v>14</v>
       </c>
       <c r="B141" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C141" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D141" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="E141">
-        <v>1</v>
+        <v>771750</v>
       </c>
       <c r="F141" t="s">
-        <v>36</v>
+        <v>17</v>
+      </c>
+      <c r="G141" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.25">
@@ -3817,16 +3820,16 @@
         <v>7</v>
       </c>
       <c r="D142" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E142">
-        <v>771750</v>
+        <v>11831218560</v>
       </c>
       <c r="F142" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G142" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.25">
@@ -3837,19 +3840,19 @@
         <v>57</v>
       </c>
       <c r="C143" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D143" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E143">
-        <v>11831218560</v>
-      </c>
-      <c r="F143" t="s">
-        <v>20</v>
+        <v>0.8</v>
+      </c>
+      <c r="F143">
+        <v>1</v>
       </c>
       <c r="G143" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.25">
@@ -3863,16 +3866,16 @@
         <v>8</v>
       </c>
       <c r="D144" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E144">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="F144">
         <v>1</v>
       </c>
       <c r="G144" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.25">
@@ -3883,19 +3886,19 @@
         <v>57</v>
       </c>
       <c r="C145" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D145" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E145">
-        <v>1</v>
-      </c>
-      <c r="F145">
-        <v>1</v>
+        <v>58</v>
+      </c>
+      <c r="F145" t="s">
+        <v>24</v>
       </c>
       <c r="G145" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.25">
@@ -3909,16 +3912,13 @@
         <v>9</v>
       </c>
       <c r="D146" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E146">
-        <v>58</v>
+        <v>5.2100000000000002E-3</v>
       </c>
       <c r="F146" t="s">
-        <v>24</v>
-      </c>
-      <c r="G146" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.25">
@@ -3929,16 +3929,16 @@
         <v>57</v>
       </c>
       <c r="C147" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D147" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="E147">
-        <v>5.2100000000000002E-3</v>
+        <v>30</v>
       </c>
       <c r="F147" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
@@ -3952,7 +3952,7 @@
         <v>10</v>
       </c>
       <c r="D148" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E148">
         <v>30</v>
@@ -3972,7 +3972,7 @@
         <v>10</v>
       </c>
       <c r="D149" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E149">
         <v>30</v>
@@ -3992,7 +3992,7 @@
         <v>10</v>
       </c>
       <c r="D150" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E150">
         <v>30</v>
@@ -4012,7 +4012,7 @@
         <v>10</v>
       </c>
       <c r="D151" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E151">
         <v>30</v>
@@ -4029,16 +4029,19 @@
         <v>57</v>
       </c>
       <c r="C152" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D152" t="s">
-        <v>32</v>
-      </c>
-      <c r="E152">
-        <v>30</v>
-      </c>
-      <c r="F152" t="s">
-        <v>28</v>
+        <v>33</v>
+      </c>
+      <c r="E152" t="s">
+        <v>51</v>
+      </c>
+      <c r="F152">
+        <v>1</v>
+      </c>
+      <c r="G152" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
@@ -4049,19 +4052,19 @@
         <v>57</v>
       </c>
       <c r="C153" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D153" t="s">
         <v>33</v>
       </c>
-      <c r="E153" t="s">
-        <v>51</v>
-      </c>
-      <c r="F153">
-        <v>1</v>
+      <c r="E153">
+        <v>2.15</v>
+      </c>
+      <c r="F153" t="s">
+        <v>34</v>
       </c>
       <c r="G153" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.25">
@@ -4072,19 +4075,16 @@
         <v>57</v>
       </c>
       <c r="C154" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D154" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E154">
-        <v>2.15</v>
+        <v>1</v>
       </c>
       <c r="F154" t="s">
-        <v>34</v>
-      </c>
-      <c r="G154" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.25">
@@ -4092,19 +4092,22 @@
         <v>14</v>
       </c>
       <c r="B155" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C155" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D155" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="E155">
-        <v>1</v>
+        <v>771750</v>
       </c>
       <c r="F155" t="s">
-        <v>36</v>
+        <v>17</v>
+      </c>
+      <c r="G155" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.25">
@@ -4118,16 +4121,16 @@
         <v>7</v>
       </c>
       <c r="D156" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E156">
-        <v>771750</v>
+        <v>10880495640</v>
       </c>
       <c r="F156" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G156" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.25">
@@ -4138,19 +4141,19 @@
         <v>58</v>
       </c>
       <c r="C157" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D157" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E157">
-        <v>10880495640</v>
-      </c>
-      <c r="F157" t="s">
-        <v>20</v>
+        <v>0.8</v>
+      </c>
+      <c r="F157">
+        <v>1</v>
       </c>
       <c r="G157" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.25">
@@ -4164,16 +4167,16 @@
         <v>8</v>
       </c>
       <c r="D158" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E158">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="F158">
         <v>1</v>
       </c>
       <c r="G158" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.25">
@@ -4184,19 +4187,19 @@
         <v>58</v>
       </c>
       <c r="C159" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D159" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E159">
-        <v>1</v>
-      </c>
-      <c r="F159">
-        <v>1</v>
+        <v>58</v>
+      </c>
+      <c r="F159" t="s">
+        <v>24</v>
       </c>
       <c r="G159" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.25">
@@ -4210,16 +4213,13 @@
         <v>9</v>
       </c>
       <c r="D160" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E160">
-        <v>58</v>
+        <v>5.2100000000000002E-3</v>
       </c>
       <c r="F160" t="s">
-        <v>24</v>
-      </c>
-      <c r="G160" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.25">
@@ -4230,16 +4230,16 @@
         <v>58</v>
       </c>
       <c r="C161" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D161" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="E161">
-        <v>5.2100000000000002E-3</v>
+        <v>30</v>
       </c>
       <c r="F161" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.25">
@@ -4253,7 +4253,7 @@
         <v>10</v>
       </c>
       <c r="D162" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E162">
         <v>30</v>
@@ -4273,7 +4273,7 @@
         <v>10</v>
       </c>
       <c r="D163" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E163">
         <v>30</v>
@@ -4293,7 +4293,7 @@
         <v>10</v>
       </c>
       <c r="D164" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E164">
         <v>30</v>
@@ -4313,7 +4313,7 @@
         <v>10</v>
       </c>
       <c r="D165" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E165">
         <v>30</v>
@@ -4330,16 +4330,19 @@
         <v>58</v>
       </c>
       <c r="C166" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D166" t="s">
-        <v>32</v>
-      </c>
-      <c r="E166">
-        <v>30</v>
-      </c>
-      <c r="F166" t="s">
-        <v>28</v>
+        <v>33</v>
+      </c>
+      <c r="E166" t="s">
+        <v>59</v>
+      </c>
+      <c r="F166">
+        <v>1</v>
+      </c>
+      <c r="G166" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.25">
@@ -4350,19 +4353,19 @@
         <v>58</v>
       </c>
       <c r="C167" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D167" t="s">
         <v>33</v>
       </c>
-      <c r="E167" t="s">
-        <v>59</v>
-      </c>
-      <c r="F167">
-        <v>1</v>
+      <c r="E167">
+        <v>2.15</v>
+      </c>
+      <c r="F167" t="s">
+        <v>34</v>
       </c>
       <c r="G167" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.25">
@@ -4373,19 +4376,16 @@
         <v>58</v>
       </c>
       <c r="C168" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D168" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E168">
-        <v>2.15</v>
+        <v>1</v>
       </c>
       <c r="F168" t="s">
-        <v>34</v>
-      </c>
-      <c r="G168" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.25">
@@ -4393,19 +4393,22 @@
         <v>14</v>
       </c>
       <c r="B169" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C169" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D169" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="E169">
-        <v>1</v>
+        <v>771750</v>
       </c>
       <c r="F169" t="s">
-        <v>36</v>
+        <v>17</v>
+      </c>
+      <c r="G169" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.25">
@@ -4419,16 +4422,16 @@
         <v>7</v>
       </c>
       <c r="D170" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E170">
-        <v>771750</v>
+        <v>10246680360</v>
       </c>
       <c r="F170" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G170" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.25">
@@ -4439,19 +4442,19 @@
         <v>60</v>
       </c>
       <c r="C171" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D171" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E171">
-        <v>10246680360</v>
-      </c>
-      <c r="F171" t="s">
-        <v>20</v>
+        <v>0.8</v>
+      </c>
+      <c r="F171">
+        <v>1</v>
       </c>
       <c r="G171" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.25">
@@ -4465,16 +4468,16 @@
         <v>8</v>
       </c>
       <c r="D172" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E172">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="F172">
         <v>1</v>
       </c>
       <c r="G172" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.25">
@@ -4485,19 +4488,19 @@
         <v>60</v>
       </c>
       <c r="C173" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D173" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E173">
-        <v>1</v>
-      </c>
-      <c r="F173">
-        <v>1</v>
+        <v>58</v>
+      </c>
+      <c r="F173" t="s">
+        <v>24</v>
       </c>
       <c r="G173" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.25">
@@ -4511,16 +4514,13 @@
         <v>9</v>
       </c>
       <c r="D174" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E174">
-        <v>58</v>
+        <v>5.2100000000000002E-3</v>
       </c>
       <c r="F174" t="s">
-        <v>24</v>
-      </c>
-      <c r="G174" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.25">
@@ -4531,16 +4531,16 @@
         <v>60</v>
       </c>
       <c r="C175" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D175" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="E175">
-        <v>5.2100000000000002E-3</v>
+        <v>30</v>
       </c>
       <c r="F175" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.25">
@@ -4554,7 +4554,7 @@
         <v>10</v>
       </c>
       <c r="D176" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E176">
         <v>30</v>
@@ -4574,7 +4574,7 @@
         <v>10</v>
       </c>
       <c r="D177" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E177">
         <v>30</v>
@@ -4594,7 +4594,7 @@
         <v>10</v>
       </c>
       <c r="D178" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E178">
         <v>30</v>
@@ -4614,7 +4614,7 @@
         <v>10</v>
       </c>
       <c r="D179" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E179">
         <v>30</v>
@@ -4631,16 +4631,19 @@
         <v>60</v>
       </c>
       <c r="C180" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D180" t="s">
-        <v>32</v>
-      </c>
-      <c r="E180">
-        <v>30</v>
-      </c>
-      <c r="F180" t="s">
-        <v>28</v>
+        <v>33</v>
+      </c>
+      <c r="E180" t="s">
+        <v>54</v>
+      </c>
+      <c r="F180">
+        <v>1</v>
+      </c>
+      <c r="G180" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.25">
@@ -4651,19 +4654,19 @@
         <v>60</v>
       </c>
       <c r="C181" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D181" t="s">
         <v>33</v>
       </c>
-      <c r="E181" t="s">
-        <v>54</v>
-      </c>
-      <c r="F181">
-        <v>1</v>
+      <c r="E181">
+        <v>2.15</v>
+      </c>
+      <c r="F181" t="s">
+        <v>34</v>
       </c>
       <c r="G181" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.25">
@@ -4674,38 +4677,15 @@
         <v>60</v>
       </c>
       <c r="C182" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D182" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E182">
-        <v>2.15</v>
+        <v>1</v>
       </c>
       <c r="F182" t="s">
-        <v>34</v>
-      </c>
-      <c r="G182" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A183" t="s">
-        <v>14</v>
-      </c>
-      <c r="B183" t="s">
-        <v>60</v>
-      </c>
-      <c r="C183" t="s">
-        <v>13</v>
-      </c>
-      <c r="D183" t="s">
-        <v>35</v>
-      </c>
-      <c r="E183">
-        <v>1</v>
-      </c>
-      <c r="F183" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>